<commit_message>
Update FORWARDED FOR PRINTING PURPOSE.xlsx
</commit_message>
<xml_diff>
--- a/18 - 2 - 2024/FORWARDED FOR PRINTING PURPOSE.xlsx
+++ b/18 - 2 - 2024/FORWARDED FOR PRINTING PURPOSE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\bashir\18 - 2 - 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0867C0DE-EE00-46C4-B070-4A2555055A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35ABCBD7-753B-4BE6-A5B0-58B723A5C735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5754EDB6-AC50-44B2-8BB6-BD21556617BD}"/>
   </bookViews>
@@ -9587,30 +9587,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDD6B5C-CAB7-4E5A-9A83-AB3221945E1E}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O627"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" style="35" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="24.5546875" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="38.109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="13.6640625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" style="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -9658,7 +9658,7 @@
       </c>
       <c r="O1" s="6"/>
     </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1292</v>
       </c>
@@ -9705,7 +9705,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1293</v>
       </c>
@@ -9752,7 +9752,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>1294</v>
       </c>
@@ -9846,7 +9846,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>1296</v>
       </c>
@@ -9940,7 +9940,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>1298</v>
       </c>
@@ -9987,7 +9987,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>1299</v>
       </c>
@@ -10034,7 +10034,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>1300</v>
       </c>
@@ -10081,7 +10081,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>1301</v>
       </c>
@@ -10128,7 +10128,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>1302</v>
       </c>
@@ -10175,7 +10175,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>1303</v>
       </c>
@@ -10269,7 +10269,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>1305</v>
       </c>
@@ -10316,7 +10316,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>1306</v>
       </c>
@@ -10363,7 +10363,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>1307</v>
       </c>
@@ -10410,7 +10410,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>1308</v>
       </c>
@@ -10455,7 +10455,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="19" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>1309</v>
       </c>
@@ -10500,7 +10500,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>1310</v>
       </c>
@@ -10547,7 +10547,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="21" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>1311</v>
       </c>
@@ -10594,7 +10594,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>1312</v>
       </c>
@@ -10639,7 +10639,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>1313</v>
       </c>
@@ -10684,7 +10684,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="24" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>1314</v>
       </c>
@@ -10729,7 +10729,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="25" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>1315</v>
       </c>
@@ -10774,7 +10774,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>1316</v>
       </c>
@@ -10866,7 +10866,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>1318</v>
       </c>
@@ -10958,7 +10958,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>1320</v>
       </c>
@@ -11003,7 +11003,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>1321</v>
       </c>
@@ -11050,7 +11050,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>1322</v>
       </c>
@@ -11095,7 +11095,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>1323</v>
       </c>
@@ -11142,7 +11142,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>1324</v>
       </c>
@@ -11189,7 +11189,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>1325</v>
       </c>
@@ -11232,7 +11232,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>1326</v>
       </c>
@@ -11277,7 +11277,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>1327</v>
       </c>
@@ -11324,7 +11324,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>1328</v>
       </c>
@@ -11371,7 +11371,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="39" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>1329</v>
       </c>
@@ -11418,7 +11418,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="40" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>1330</v>
       </c>
@@ -11463,7 +11463,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="41" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>1331</v>
       </c>
@@ -11508,7 +11508,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="42" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>1332</v>
       </c>
@@ -11600,7 +11600,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="44" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>1334</v>
       </c>
@@ -11645,7 +11645,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="45" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>1335</v>
       </c>
@@ -11692,7 +11692,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="46" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>1336</v>
       </c>
@@ -11735,7 +11735,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="47" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>1337</v>
       </c>
@@ -11782,7 +11782,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="48" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>1338</v>
       </c>
@@ -11829,7 +11829,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="49" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>1339</v>
       </c>
@@ -11876,7 +11876,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="50" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>1340</v>
       </c>
@@ -11923,7 +11923,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>1341</v>
       </c>
@@ -11970,7 +11970,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="52" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>1342</v>
       </c>
@@ -12017,7 +12017,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>1343</v>
       </c>
@@ -12111,7 +12111,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="55" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>1345</v>
       </c>
@@ -12158,7 +12158,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="56" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>1346</v>
       </c>
@@ -12205,7 +12205,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="57" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>1347</v>
       </c>
@@ -12252,7 +12252,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="58" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>1348</v>
       </c>
@@ -12391,7 +12391,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="61" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>1351</v>
       </c>
@@ -12483,7 +12483,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="63" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>1353</v>
       </c>
@@ -12577,7 +12577,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="65" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>1355</v>
       </c>
@@ -12624,7 +12624,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="66" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>1356</v>
       </c>
@@ -12669,7 +12669,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="67" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>1357</v>
       </c>
@@ -12716,7 +12716,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="68" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>1358</v>
       </c>
@@ -12761,7 +12761,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="69" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>1359</v>
       </c>
@@ -12808,7 +12808,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="70" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>1360</v>
       </c>
@@ -12855,7 +12855,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="71" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>1361</v>
       </c>
@@ -12902,7 +12902,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="72" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>1362</v>
       </c>
@@ -12949,7 +12949,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="73" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>1363</v>
       </c>
@@ -13043,7 +13043,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="75" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>1365</v>
       </c>
@@ -13090,7 +13090,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="76" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>1366</v>
       </c>
@@ -13137,7 +13137,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="77" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>1367</v>
       </c>
@@ -13182,7 +13182,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="78" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>1368</v>
       </c>
@@ -13229,7 +13229,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="79" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>1369</v>
       </c>
@@ -13276,7 +13276,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="80" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>1370</v>
       </c>
@@ -13323,7 +13323,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="81" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>1371</v>
       </c>
@@ -13368,7 +13368,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="82" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>1372</v>
       </c>
@@ -13415,7 +13415,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="83" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>1373</v>
       </c>
@@ -13462,7 +13462,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="84" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
         <v>1374</v>
       </c>
@@ -13507,7 +13507,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="85" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>1375</v>
       </c>
@@ -13554,7 +13554,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="86" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>1376</v>
       </c>
@@ -13599,7 +13599,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="87" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>1377</v>
       </c>
@@ -13646,7 +13646,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="88" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>1378</v>
       </c>
@@ -13691,7 +13691,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="89" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
         <v>1379</v>
       </c>
@@ -13738,7 +13738,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="90" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>1380</v>
       </c>
@@ -13783,7 +13783,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="91" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
         <v>1381</v>
       </c>
@@ -13828,7 +13828,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="92" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>1382</v>
       </c>
@@ -13873,7 +13873,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="93" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
         <v>1383</v>
       </c>
@@ -13920,7 +13920,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="94" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>1384</v>
       </c>
@@ -13965,7 +13965,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="95" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
         <v>1385</v>
       </c>
@@ -14012,7 +14012,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="96" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>1386</v>
       </c>
@@ -14106,7 +14106,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="98" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>1388</v>
       </c>
@@ -14153,7 +14153,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="99" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
         <v>1389</v>
       </c>
@@ -14200,7 +14200,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="100" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
         <v>1390</v>
       </c>
@@ -14245,7 +14245,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="101" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
         <v>1391</v>
       </c>
@@ -14292,7 +14292,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="102" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
         <v>1392</v>
       </c>
@@ -14339,7 +14339,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="103" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
         <v>1393</v>
       </c>
@@ -14386,7 +14386,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="104" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
         <v>1394</v>
       </c>
@@ -14433,7 +14433,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="105" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
         <v>1395</v>
       </c>
@@ -14480,7 +14480,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="106" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
         <v>1396</v>
       </c>
@@ -14525,7 +14525,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="107" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4">
         <v>1397</v>
       </c>
@@ -14570,7 +14570,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="108" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
         <v>1398</v>
       </c>
@@ -14703,7 +14703,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="111" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
         <v>1401</v>
       </c>
@@ -14750,7 +14750,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="112" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
         <v>1402</v>
       </c>
@@ -14797,7 +14797,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="113" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4">
         <v>1403</v>
       </c>
@@ -14842,7 +14842,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="114" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4">
         <v>1404</v>
       </c>
@@ -14889,7 +14889,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="115" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="4">
         <v>1405</v>
       </c>
@@ -14934,7 +14934,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="116" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="4">
         <v>1406</v>
       </c>
@@ -14981,7 +14981,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="117" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="4">
         <v>1407</v>
       </c>
@@ -15028,7 +15028,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="118" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="4">
         <v>1408</v>
       </c>
@@ -15073,7 +15073,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="119" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="4">
         <v>1409</v>
       </c>
@@ -15120,7 +15120,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="120" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="4">
         <v>1410</v>
       </c>
@@ -15165,7 +15165,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="121" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="4">
         <v>1411</v>
       </c>
@@ -15212,7 +15212,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="122" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="4">
         <v>1412</v>
       </c>
@@ -15259,7 +15259,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="123" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="4">
         <v>1413</v>
       </c>
@@ -15306,7 +15306,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="124" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="4">
         <v>1414</v>
       </c>
@@ -15353,7 +15353,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="125" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="4">
         <v>1415</v>
       </c>
@@ -15400,7 +15400,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="126" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="4">
         <v>1416</v>
       </c>
@@ -15494,7 +15494,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="128" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="4">
         <v>1418</v>
       </c>
@@ -15541,7 +15541,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="129" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="4">
         <v>1419</v>
       </c>
@@ -15586,7 +15586,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="130" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="4">
         <v>1420</v>
       </c>
@@ -15633,7 +15633,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="131" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="4">
         <v>1421</v>
       </c>
@@ -15680,7 +15680,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="132" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="4">
         <v>1422</v>
       </c>
@@ -15727,7 +15727,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="133" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="4">
         <v>1423</v>
       </c>
@@ -15772,7 +15772,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="134" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4">
         <v>1424</v>
       </c>
@@ -15819,7 +15819,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="135" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="4">
         <v>1425</v>
       </c>
@@ -15862,7 +15862,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="136" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="4">
         <v>1426</v>
       </c>
@@ -15909,7 +15909,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="137" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="4">
         <v>1427</v>
       </c>
@@ -15956,7 +15956,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="138" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="4">
         <v>1428</v>
       </c>
@@ -16003,7 +16003,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="139" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="4">
         <v>1429</v>
       </c>
@@ -16048,7 +16048,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="140" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="4">
         <v>1430</v>
       </c>
@@ -16095,7 +16095,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="141" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="4">
         <v>1431</v>
       </c>
@@ -16142,7 +16142,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="142" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="4">
         <v>1432</v>
       </c>
@@ -16187,7 +16187,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="143" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="4">
         <v>1433</v>
       </c>
@@ -16234,7 +16234,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="144" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="4">
         <v>1434</v>
       </c>
@@ -16281,7 +16281,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="145" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="4">
         <v>1435</v>
       </c>
@@ -16326,7 +16326,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="146" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="4">
         <v>1436</v>
       </c>
@@ -16373,7 +16373,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="147" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="4">
         <v>1437</v>
       </c>
@@ -16418,7 +16418,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="148" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="4">
         <v>1438</v>
       </c>
@@ -16465,7 +16465,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="149" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="4">
         <v>1439</v>
       </c>
@@ -16512,7 +16512,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="150" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="4">
         <v>1440</v>
       </c>
@@ -16559,7 +16559,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="151" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="4">
         <v>1441</v>
       </c>
@@ -16604,7 +16604,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="152" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="4">
         <v>1442</v>
       </c>
@@ -16651,7 +16651,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="153" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="4">
         <v>1443</v>
       </c>
@@ -16698,7 +16698,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="154" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="4">
         <v>1444</v>
       </c>
@@ -16743,7 +16743,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="155" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="4">
         <v>1445</v>
       </c>
@@ -16788,7 +16788,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="156" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="4">
         <v>1446</v>
       </c>
@@ -16835,7 +16835,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="157" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="4">
         <v>1447</v>
       </c>
@@ -16882,7 +16882,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="158" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="4">
         <v>1448</v>
       </c>
@@ -16927,7 +16927,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="159" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="4">
         <v>1449</v>
       </c>
@@ -17019,7 +17019,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="161" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="4">
         <v>1451</v>
       </c>
@@ -17064,7 +17064,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="162" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="4">
         <v>1452</v>
       </c>
@@ -17111,7 +17111,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="163" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="4">
         <v>1453</v>
       </c>
@@ -17154,7 +17154,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="164" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="4">
         <v>1454</v>
       </c>
@@ -17201,7 +17201,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="165" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="4">
         <v>1455</v>
       </c>
@@ -17248,7 +17248,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="166" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="4">
         <v>1456</v>
       </c>
@@ -17295,7 +17295,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="167" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="4">
         <v>1457</v>
       </c>
@@ -17342,7 +17342,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="168" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="4">
         <v>1458</v>
       </c>
@@ -17389,7 +17389,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="169" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="4">
         <v>1459</v>
       </c>
@@ -17434,7 +17434,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="170" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="4">
         <v>1460</v>
       </c>
@@ -17481,7 +17481,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="171" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="4">
         <v>1461</v>
       </c>
@@ -17526,7 +17526,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="172" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="4">
         <v>1462</v>
       </c>
@@ -17573,7 +17573,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="173" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="4">
         <v>1463</v>
       </c>
@@ -17620,7 +17620,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="174" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="4">
         <v>1464</v>
       </c>
@@ -17667,7 +17667,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="175" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="4">
         <v>1465</v>
       </c>
@@ -17714,7 +17714,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="176" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="4">
         <v>1466</v>
       </c>
@@ -17761,7 +17761,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="177" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="4">
         <v>1467</v>
       </c>
@@ -17806,7 +17806,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="178" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="4">
         <v>1468</v>
       </c>
@@ -17853,7 +17853,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="179" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="4">
         <v>1469</v>
       </c>
@@ -17900,7 +17900,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="180" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="4">
         <v>1470</v>
       </c>
@@ -17947,7 +17947,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="181" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="4">
         <v>1471</v>
       </c>
@@ -17994,7 +17994,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="182" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="4">
         <v>1472</v>
       </c>
@@ -18088,7 +18088,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="184" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="4">
         <v>1474</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="186" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="4">
         <v>1476</v>
       </c>
@@ -18270,7 +18270,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="188" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="4">
         <v>1478</v>
       </c>
@@ -18317,7 +18317,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="189" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="4">
         <v>1479</v>
       </c>
@@ -18364,7 +18364,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="190" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="4">
         <v>1480</v>
       </c>
@@ -18411,7 +18411,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="191" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="4">
         <v>1481</v>
       </c>
@@ -18505,7 +18505,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="193" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="4">
         <v>1483</v>
       </c>
@@ -18599,7 +18599,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="195" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="4">
         <v>1485</v>
       </c>
@@ -18691,7 +18691,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="197" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="4">
         <v>1487</v>
       </c>
@@ -18785,7 +18785,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="199" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="4">
         <v>1489</v>
       </c>
@@ -18832,7 +18832,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="200" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="4">
         <v>1490</v>
       </c>
@@ -18879,7 +18879,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="201" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="4">
         <v>1491</v>
       </c>
@@ -18924,7 +18924,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="202" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="4">
         <v>1492</v>
       </c>
@@ -18971,7 +18971,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="203" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="4">
         <v>1493</v>
       </c>
@@ -19018,7 +19018,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="204" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="4">
         <v>1494</v>
       </c>
@@ -19065,7 +19065,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="205" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="4">
         <v>1495</v>
       </c>
@@ -19159,7 +19159,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="207" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="4">
         <v>1497</v>
       </c>
@@ -19206,7 +19206,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="208" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="4">
         <v>1498</v>
       </c>
@@ -19253,7 +19253,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="209" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="4">
         <v>1499</v>
       </c>
@@ -19300,7 +19300,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="210" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="4">
         <v>1500</v>
       </c>
@@ -19347,7 +19347,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="211" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="4">
         <v>1501</v>
       </c>
@@ -19394,7 +19394,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="212" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="4">
         <v>1502</v>
       </c>
@@ -19441,7 +19441,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="213" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="4">
         <v>1503</v>
       </c>
@@ -19486,7 +19486,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="214" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="4">
         <v>1504</v>
       </c>
@@ -19531,7 +19531,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="215" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="4">
         <v>1505</v>
       </c>
@@ -19578,7 +19578,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="216" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="4">
         <v>1506</v>
       </c>
@@ -19625,7 +19625,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="217" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="4">
         <v>1507</v>
       </c>
@@ -19672,7 +19672,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="218" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="4">
         <v>1508</v>
       </c>
@@ -19719,7 +19719,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="219" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="4">
         <v>1509</v>
       </c>
@@ -19766,7 +19766,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="220" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="4">
         <v>1510</v>
       </c>
@@ -19813,7 +19813,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="221" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="4">
         <v>1511</v>
       </c>
@@ -19860,7 +19860,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="222" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="4">
         <v>1512</v>
       </c>
@@ -19907,7 +19907,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="223" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="4">
         <v>1513</v>
       </c>
@@ -19954,7 +19954,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="224" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="4">
         <v>1514</v>
       </c>
@@ -20001,7 +20001,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="225" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="4">
         <v>1515</v>
       </c>
@@ -20095,7 +20095,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="227" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="4">
         <v>1517</v>
       </c>
@@ -20189,7 +20189,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="229" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="4">
         <v>1519</v>
       </c>
@@ -20236,7 +20236,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="230" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="4">
         <v>1520</v>
       </c>
@@ -20328,7 +20328,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="232" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="4">
         <v>1522</v>
       </c>
@@ -20375,7 +20375,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="233" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="4">
         <v>1523</v>
       </c>
@@ -20422,7 +20422,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="234" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="4">
         <v>1524</v>
       </c>
@@ -20469,7 +20469,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="235" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="4">
         <v>1525</v>
       </c>
@@ -20516,7 +20516,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="236" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="4">
         <v>1526</v>
       </c>
@@ -20563,7 +20563,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="237" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="4">
         <v>1527</v>
       </c>
@@ -20608,7 +20608,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="238" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="4">
         <v>1528</v>
       </c>
@@ -20655,7 +20655,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="239" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="4">
         <v>1529</v>
       </c>
@@ -20702,7 +20702,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="240" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="4">
         <v>1530</v>
       </c>
@@ -20749,7 +20749,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="241" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="4">
         <v>1531</v>
       </c>
@@ -20796,7 +20796,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="242" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="4">
         <v>1532</v>
       </c>
@@ -20843,7 +20843,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="243" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="4">
         <v>1533</v>
       </c>
@@ -20890,7 +20890,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="244" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="4">
         <v>1534</v>
       </c>
@@ -20935,7 +20935,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="245" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="4">
         <v>1535</v>
       </c>
@@ -20980,7 +20980,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="246" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="4">
         <v>1536</v>
       </c>
@@ -21027,7 +21027,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="247" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="4">
         <v>1537</v>
       </c>
@@ -21074,7 +21074,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="248" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="4">
         <v>1538</v>
       </c>
@@ -21121,7 +21121,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="249" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="4">
         <v>1539</v>
       </c>
@@ -21260,7 +21260,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="252" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="4">
         <v>1542</v>
       </c>
@@ -21307,7 +21307,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="253" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="4">
         <v>1543</v>
       </c>
@@ -21354,7 +21354,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="254" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="4">
         <v>1544</v>
       </c>
@@ -21448,7 +21448,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="256" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="4">
         <v>1546</v>
       </c>
@@ -21495,7 +21495,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="257" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="4">
         <v>1547</v>
       </c>
@@ -21542,7 +21542,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="258" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="4">
         <v>1548</v>
       </c>
@@ -21589,7 +21589,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="259" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="4">
         <v>1549</v>
       </c>
@@ -21636,7 +21636,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="260" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="4">
         <v>1550</v>
       </c>
@@ -21681,7 +21681,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="261" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="4">
         <v>1551</v>
       </c>
@@ -21775,7 +21775,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="263" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="4">
         <v>1553</v>
       </c>
@@ -21822,7 +21822,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="264" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="4">
         <v>1554</v>
       </c>
@@ -21916,7 +21916,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="266" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="4">
         <v>1556</v>
       </c>
@@ -21963,7 +21963,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="267" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="4">
         <v>1557</v>
       </c>
@@ -22057,7 +22057,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="269" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="4">
         <v>1559</v>
       </c>
@@ -22104,7 +22104,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="270" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="4">
         <v>1560</v>
       </c>
@@ -22198,7 +22198,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="272" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" s="4">
         <v>1562</v>
       </c>
@@ -22245,7 +22245,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="273" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="4">
         <v>1563</v>
       </c>
@@ -22288,7 +22288,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="274" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="4">
         <v>1564</v>
       </c>
@@ -22335,7 +22335,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="275" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="4">
         <v>1565</v>
       </c>
@@ -22382,7 +22382,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="276" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="4">
         <v>1566</v>
       </c>
@@ -22474,7 +22474,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="278" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="4">
         <v>1568</v>
       </c>
@@ -22521,7 +22521,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="279" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="4">
         <v>1569</v>
       </c>
@@ -22566,7 +22566,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="280" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="4">
         <v>1570</v>
       </c>
@@ -22613,7 +22613,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="281" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="4">
         <v>1571</v>
       </c>
@@ -22707,7 +22707,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="283" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" s="4">
         <v>1573</v>
       </c>
@@ -22754,7 +22754,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="284" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" s="4">
         <v>1574</v>
       </c>
@@ -22801,7 +22801,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="285" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" s="4">
         <v>1575</v>
       </c>
@@ -22848,7 +22848,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="286" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="4">
         <v>1576</v>
       </c>
@@ -22940,7 +22940,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="288" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="4">
         <v>1578</v>
       </c>
@@ -23081,7 +23081,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="291" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" s="4">
         <v>1581</v>
       </c>
@@ -23173,7 +23173,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="293" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="4">
         <v>1583</v>
       </c>
@@ -23265,7 +23265,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="295" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" s="4">
         <v>1585</v>
       </c>
@@ -23312,7 +23312,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="296" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" s="4">
         <v>1586</v>
       </c>
@@ -23406,7 +23406,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="298" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A298" s="4">
         <v>1588</v>
       </c>
@@ -23500,7 +23500,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="300" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" s="4">
         <v>1590</v>
       </c>
@@ -23688,7 +23688,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="304" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" s="4">
         <v>1594</v>
       </c>
@@ -23923,7 +23923,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="309" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="4">
         <v>1599</v>
       </c>
@@ -23970,7 +23970,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="310" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A310" s="4">
         <v>1600</v>
       </c>
@@ -24017,7 +24017,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="311" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" s="4">
         <v>1601</v>
       </c>
@@ -24064,7 +24064,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="312" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A312" s="4">
         <v>1602</v>
       </c>
@@ -24111,7 +24111,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="313" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A313" s="4">
         <v>1603</v>
       </c>
@@ -24205,7 +24205,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="315" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A315" s="4">
         <v>1605</v>
       </c>
@@ -24297,7 +24297,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="317" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A317" s="4">
         <v>1607</v>
       </c>
@@ -24344,7 +24344,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="318" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A318" s="4">
         <v>1608</v>
       </c>
@@ -24391,7 +24391,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="319" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A319" s="4">
         <v>1609</v>
       </c>
@@ -24485,7 +24485,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="321" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A321" s="4">
         <v>1611</v>
       </c>
@@ -24577,7 +24577,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="323" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" s="4">
         <v>1613</v>
       </c>
@@ -24624,7 +24624,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="324" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A324" s="4">
         <v>1614</v>
       </c>
@@ -24671,7 +24671,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="325" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A325" s="4">
         <v>1615</v>
       </c>
@@ -24718,7 +24718,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="326" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A326" s="4">
         <v>1616</v>
       </c>
@@ -24763,7 +24763,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="327" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A327" s="4">
         <v>1617</v>
       </c>
@@ -24808,7 +24808,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="328" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A328" s="4">
         <v>1618</v>
       </c>
@@ -24853,7 +24853,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="329" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A329" s="4">
         <v>1619</v>
       </c>
@@ -24898,7 +24898,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="330" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A330" s="4">
         <v>1620</v>
       </c>
@@ -24945,7 +24945,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="331" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A331" s="4">
         <v>1621</v>
       </c>
@@ -24992,7 +24992,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="332" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A332" s="4">
         <v>1622</v>
       </c>
@@ -25039,7 +25039,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="333" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A333" s="4">
         <v>1623</v>
       </c>
@@ -25084,7 +25084,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="334" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A334" s="4">
         <v>1624</v>
       </c>
@@ -25129,7 +25129,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="335" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A335" s="4">
         <v>1625</v>
       </c>
@@ -25176,7 +25176,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="336" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A336" s="4">
         <v>1626</v>
       </c>
@@ -25223,7 +25223,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="337" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A337" s="4">
         <v>1627</v>
       </c>
@@ -25315,7 +25315,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="339" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A339" s="4">
         <v>1629</v>
       </c>
@@ -25362,7 +25362,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="340" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A340" s="4">
         <v>1630</v>
       </c>
@@ -25407,7 +25407,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="341" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A341" s="4">
         <v>1631</v>
       </c>
@@ -25454,7 +25454,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="342" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A342" s="4">
         <v>1632</v>
       </c>
@@ -25499,7 +25499,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="343" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A343" s="4">
         <v>1633</v>
       </c>
@@ -25546,7 +25546,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="344" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A344" s="4">
         <v>1634</v>
       </c>
@@ -25687,7 +25687,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="347" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A347" s="4">
         <v>1637</v>
       </c>
@@ -25828,7 +25828,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="350" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A350" s="4">
         <v>1640</v>
       </c>
@@ -25875,7 +25875,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="351" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A351" s="4">
         <v>1641</v>
       </c>
@@ -25922,7 +25922,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="352" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A352" s="4">
         <v>1642</v>
       </c>
@@ -26016,7 +26016,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="354" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A354" s="4">
         <v>1644</v>
       </c>
@@ -26063,7 +26063,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="355" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A355" s="4">
         <v>1645</v>
       </c>
@@ -26202,7 +26202,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="358" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A358" s="4">
         <v>1648</v>
       </c>
@@ -26249,7 +26249,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="359" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A359" s="4">
         <v>1649</v>
       </c>
@@ -26296,7 +26296,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="360" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A360" s="4">
         <v>1650</v>
       </c>
@@ -26388,7 +26388,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="362" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A362" s="4">
         <v>1652</v>
       </c>
@@ -26482,7 +26482,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="364" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A364" s="4">
         <v>1654</v>
       </c>
@@ -26527,7 +26527,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="365" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A365" s="4">
         <v>1655</v>
       </c>
@@ -26621,7 +26621,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="367" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A367" s="4">
         <v>1657</v>
       </c>
@@ -26668,7 +26668,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="368" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A368" s="4">
         <v>1658</v>
       </c>
@@ -26715,7 +26715,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="369" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A369" s="4">
         <v>1659</v>
       </c>
@@ -26807,7 +26807,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="371" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A371" s="4">
         <v>1661</v>
       </c>
@@ -26854,7 +26854,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="372" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A372" s="4">
         <v>1662</v>
       </c>
@@ -26901,7 +26901,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="373" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A373" s="4">
         <v>1663</v>
       </c>
@@ -26948,7 +26948,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="374" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A374" s="4">
         <v>1664</v>
       </c>
@@ -27042,7 +27042,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="376" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A376" s="4">
         <v>1666</v>
       </c>
@@ -27089,7 +27089,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="377" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A377" s="4">
         <v>1667</v>
       </c>
@@ -27136,7 +27136,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="378" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A378" s="4">
         <v>1668</v>
       </c>
@@ -27230,7 +27230,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="380" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A380" s="4">
         <v>1670</v>
       </c>
@@ -27277,7 +27277,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="381" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A381" s="4">
         <v>1671</v>
       </c>
@@ -27324,7 +27324,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="382" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A382" s="4">
         <v>1672</v>
       </c>
@@ -27371,7 +27371,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="383" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A383" s="4">
         <v>1673</v>
       </c>
@@ -27465,7 +27465,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="385" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A385" s="4">
         <v>1675</v>
       </c>
@@ -27512,7 +27512,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="386" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A386" s="4">
         <v>1676</v>
       </c>
@@ -27559,7 +27559,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="387" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A387" s="4">
         <v>1677</v>
       </c>
@@ -27653,7 +27653,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="389" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A389" s="4">
         <v>1679</v>
       </c>
@@ -27700,7 +27700,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="390" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A390" s="4">
         <v>1680</v>
       </c>
@@ -27747,7 +27747,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="391" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A391" s="4">
         <v>1681</v>
       </c>
@@ -27794,7 +27794,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="392" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A392" s="4">
         <v>1682</v>
       </c>
@@ -27841,7 +27841,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="393" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A393" s="4">
         <v>1683</v>
       </c>
@@ -27888,7 +27888,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="394" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A394" s="4">
         <v>1684</v>
       </c>
@@ -27933,7 +27933,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="395" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A395" s="4">
         <v>1685</v>
       </c>
@@ -27980,7 +27980,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="396" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A396" s="4">
         <v>1686</v>
       </c>
@@ -28027,7 +28027,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="397" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A397" s="4">
         <v>1687</v>
       </c>
@@ -28119,7 +28119,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="399" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A399" s="4">
         <v>1689</v>
       </c>
@@ -28166,7 +28166,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="400" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A400" s="4">
         <v>1690</v>
       </c>
@@ -28211,7 +28211,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="401" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A401" s="4">
         <v>1691</v>
       </c>
@@ -28258,7 +28258,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="402" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A402" s="4">
         <v>1692</v>
       </c>
@@ -28305,7 +28305,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="403" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A403" s="4">
         <v>1693</v>
       </c>
@@ -28352,7 +28352,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="404" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A404" s="4">
         <v>1694</v>
       </c>
@@ -28399,7 +28399,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="405" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A405" s="4">
         <v>1695</v>
       </c>
@@ -28493,7 +28493,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="407" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A407" s="4">
         <v>1697</v>
       </c>
@@ -28540,7 +28540,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="408" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A408" s="4">
         <v>1698</v>
       </c>
@@ -28585,7 +28585,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="409" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A409" s="4">
         <v>1699</v>
       </c>
@@ -28632,7 +28632,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="410" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A410" s="4">
         <v>1700</v>
       </c>
@@ -28679,7 +28679,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="411" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A411" s="4">
         <v>1701</v>
       </c>
@@ -28726,7 +28726,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="412" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A412" s="4">
         <v>1702</v>
       </c>
@@ -28773,7 +28773,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="413" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A413" s="4">
         <v>1703</v>
       </c>
@@ -28820,7 +28820,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="414" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A414" s="4">
         <v>1704</v>
       </c>
@@ -28865,7 +28865,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="415" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A415" s="4">
         <v>1705</v>
       </c>
@@ -28912,7 +28912,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="416" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A416" s="4">
         <v>1706</v>
       </c>
@@ -28959,7 +28959,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="417" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A417" s="4">
         <v>1707</v>
       </c>
@@ -29006,7 +29006,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="418" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A418" s="4">
         <v>1708</v>
       </c>
@@ -29051,7 +29051,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="419" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A419" s="4">
         <v>1709</v>
       </c>
@@ -29096,7 +29096,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="420" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A420" s="4">
         <v>1710</v>
       </c>
@@ -29190,7 +29190,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="422" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A422" s="4">
         <v>1712</v>
       </c>
@@ -29235,7 +29235,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="423" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A423" s="4">
         <v>1713</v>
       </c>
@@ -29282,7 +29282,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="424" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A424" s="4">
         <v>1714</v>
       </c>
@@ -29376,7 +29376,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="426" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A426" s="4">
         <v>1716</v>
       </c>
@@ -29423,7 +29423,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="427" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A427" s="4">
         <v>1717</v>
       </c>
@@ -29468,7 +29468,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="428" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A428" s="4">
         <v>1718</v>
       </c>
@@ -29515,7 +29515,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="429" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A429" s="4">
         <v>1719</v>
       </c>
@@ -29562,7 +29562,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="430" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A430" s="4">
         <v>1720</v>
       </c>
@@ -29609,7 +29609,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="431" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A431" s="4">
         <v>1721</v>
       </c>
@@ -29703,7 +29703,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="433" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A433" s="4">
         <v>1723</v>
       </c>
@@ -29750,7 +29750,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="434" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A434" s="4">
         <v>1724</v>
       </c>
@@ -29842,7 +29842,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="436" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A436" s="4">
         <v>1726</v>
       </c>
@@ -29936,7 +29936,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="438" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A438" s="4">
         <v>1728</v>
       </c>
@@ -29983,7 +29983,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="439" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A439" s="4">
         <v>1729</v>
       </c>
@@ -30124,7 +30124,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="442" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A442" s="4">
         <v>1732</v>
       </c>
@@ -30216,7 +30216,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="444" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A444" s="4">
         <v>1734</v>
       </c>
@@ -30263,7 +30263,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="445" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A445" s="4">
         <v>1735</v>
       </c>
@@ -30308,7 +30308,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="446" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A446" s="4">
         <v>1736</v>
       </c>
@@ -30355,7 +30355,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="447" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A447" s="4">
         <v>1737</v>
       </c>
@@ -30400,7 +30400,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="448" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A448" s="4">
         <v>1738</v>
       </c>
@@ -30445,7 +30445,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="449" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A449" s="4">
         <v>1739</v>
       </c>
@@ -30535,7 +30535,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="451" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A451" s="4">
         <v>1741</v>
       </c>
@@ -30580,7 +30580,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="452" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A452" s="4">
         <v>1742</v>
       </c>
@@ -30672,7 +30672,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="454" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A454" s="4">
         <v>1744</v>
       </c>
@@ -30719,7 +30719,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="455" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A455" s="4">
         <v>1745</v>
       </c>
@@ -30811,7 +30811,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="457" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A457" s="4">
         <v>1747</v>
       </c>
@@ -30854,7 +30854,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="458" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A458" s="4">
         <v>1748</v>
       </c>
@@ -30946,7 +30946,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="460" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A460" s="4">
         <v>1750</v>
       </c>
@@ -30993,7 +30993,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="461" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A461" s="4">
         <v>1751</v>
       </c>
@@ -31040,7 +31040,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="462" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A462" s="4">
         <v>1752</v>
       </c>
@@ -31087,7 +31087,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="463" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A463" s="4">
         <v>1753</v>
       </c>
@@ -31132,7 +31132,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="464" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A464" s="4">
         <v>1754</v>
       </c>
@@ -31177,7 +31177,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="465" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A465" s="4">
         <v>1755</v>
       </c>
@@ -31222,7 +31222,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="466" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A466" s="4">
         <v>1756</v>
       </c>
@@ -31269,7 +31269,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="467" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A467" s="4">
         <v>1757</v>
       </c>
@@ -31316,7 +31316,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="468" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A468" s="4">
         <v>1758</v>
       </c>
@@ -31363,7 +31363,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="469" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A469" s="4">
         <v>1759</v>
       </c>
@@ -31410,7 +31410,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="470" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A470" s="4">
         <v>1760</v>
       </c>
@@ -31457,7 +31457,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="471" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A471" s="4">
         <v>1761</v>
       </c>
@@ -31551,7 +31551,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="473" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A473" s="4">
         <v>1763</v>
       </c>
@@ -31598,7 +31598,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="474" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A474" s="4">
         <v>1764</v>
       </c>
@@ -31690,7 +31690,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="476" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A476" s="4">
         <v>1766</v>
       </c>
@@ -31737,7 +31737,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="477" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A477" s="4">
         <v>1767</v>
       </c>
@@ -31784,7 +31784,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="478" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A478" s="4">
         <v>1768</v>
       </c>
@@ -31831,7 +31831,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="479" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A479" s="4">
         <v>1769</v>
       </c>
@@ -31878,7 +31878,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="480" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A480" s="4">
         <v>1770</v>
       </c>
@@ -31925,7 +31925,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="481" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A481" s="4">
         <v>1771</v>
       </c>
@@ -31972,7 +31972,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="482" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A482" s="4">
         <v>1772</v>
       </c>
@@ -32019,7 +32019,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="483" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A483" s="4">
         <v>1773</v>
       </c>
@@ -32064,7 +32064,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="484" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A484" s="4">
         <v>1774</v>
       </c>
@@ -32111,7 +32111,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="485" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A485" s="4">
         <v>1775</v>
       </c>
@@ -32156,7 +32156,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="486" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A486" s="4">
         <v>1776</v>
       </c>
@@ -32203,7 +32203,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="487" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A487" s="4">
         <v>1777</v>
       </c>
@@ -32248,7 +32248,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="488" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A488" s="4">
         <v>1778</v>
       </c>
@@ -32295,7 +32295,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="489" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A489" s="4">
         <v>1779</v>
       </c>
@@ -32342,7 +32342,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="490" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A490" s="4">
         <v>1780</v>
       </c>
@@ -32389,7 +32389,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="491" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A491" s="4">
         <v>1781</v>
       </c>
@@ -32436,7 +32436,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="492" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A492" s="4">
         <v>1782</v>
       </c>
@@ -32530,7 +32530,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="494" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A494" s="4">
         <v>1784</v>
       </c>
@@ -32577,7 +32577,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="495" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A495" s="4">
         <v>1785</v>
       </c>
@@ -32622,7 +32622,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="496" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A496" s="4">
         <v>1786</v>
       </c>
@@ -32669,7 +32669,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="497" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A497" s="4">
         <v>1787</v>
       </c>
@@ -32714,7 +32714,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="498" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A498" s="4">
         <v>1788</v>
       </c>
@@ -32757,7 +32757,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="499" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A499" s="4">
         <v>1789</v>
       </c>
@@ -32804,7 +32804,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="500" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A500" s="4">
         <v>1790</v>
       </c>
@@ -32851,7 +32851,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="501" spans="1:15" s="31" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:15" s="31" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A501" s="26">
         <v>1791</v>
       </c>
@@ -32892,7 +32892,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="502" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A502" s="4">
         <v>1792</v>
       </c>
@@ -32935,7 +32935,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="503" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A503" s="4">
         <v>1793</v>
       </c>
@@ -32978,7 +32978,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="504" spans="1:15" s="31" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:15" s="31" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A504" s="26">
         <v>1794</v>
       </c>
@@ -33021,7 +33021,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="505" spans="1:15" s="31" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:15" s="31" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A505" s="26">
         <v>1795</v>
       </c>
@@ -33064,7 +33064,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="506" spans="1:15" s="31" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:15" s="31" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A506" s="26">
         <v>1796</v>
       </c>
@@ -33107,7 +33107,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="507" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A507" s="4">
         <v>1797</v>
       </c>
@@ -33148,7 +33148,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="508" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A508" s="4">
         <v>1798</v>
       </c>
@@ -33189,7 +33189,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="509" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A509" s="4">
         <v>1799</v>
       </c>
@@ -33232,7 +33232,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="510" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A510" s="4">
         <v>1800</v>
       </c>
@@ -33277,7 +33277,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="511" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A511" s="4">
         <v>1801</v>
       </c>
@@ -33371,7 +33371,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="513" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A513" s="4">
         <v>1803</v>
       </c>
@@ -33418,7 +33418,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="514" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A514" s="4">
         <v>1804</v>
       </c>
@@ -33465,7 +33465,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="515" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A515" s="4">
         <v>1805</v>
       </c>
@@ -33557,7 +33557,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="517" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A517" s="4">
         <v>1807</v>
       </c>
@@ -33604,7 +33604,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="518" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A518" s="4">
         <v>1808</v>
       </c>
@@ -33651,7 +33651,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="519" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A519" s="4">
         <v>1809</v>
       </c>
@@ -33698,7 +33698,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="520" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A520" s="4">
         <v>1810</v>
       </c>
@@ -33745,7 +33745,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="521" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="521" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A521" s="4">
         <v>1811</v>
       </c>
@@ -33792,7 +33792,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="522" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A522" s="4">
         <v>1812</v>
       </c>
@@ -33839,7 +33839,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="523" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="523" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A523" s="4">
         <v>1813</v>
       </c>
@@ -33886,7 +33886,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="524" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A524" s="4">
         <v>1814</v>
       </c>
@@ -33933,7 +33933,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="525" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A525" s="4">
         <v>1815</v>
       </c>
@@ -33980,7 +33980,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="526" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="526" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A526" s="4">
         <v>1816</v>
       </c>
@@ -34105,7 +34105,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="529" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A529" s="4">
         <v>1819</v>
       </c>
@@ -34152,7 +34152,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="530" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="530" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A530" s="4">
         <v>1820</v>
       </c>
@@ -34236,7 +34236,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="532" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A532" s="4">
         <v>1822</v>
       </c>
@@ -34283,7 +34283,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="533" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A533" s="4">
         <v>1823</v>
       </c>
@@ -34330,7 +34330,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="534" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A534" s="4">
         <v>1824</v>
       </c>
@@ -34377,7 +34377,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="535" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="535" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A535" s="4">
         <v>1825</v>
       </c>
@@ -34424,7 +34424,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="536" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="536" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A536" s="4">
         <v>1826</v>
       </c>
@@ -34471,7 +34471,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="537" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A537" s="4">
         <v>1827</v>
       </c>
@@ -34516,7 +34516,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="538" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A538" s="4">
         <v>1828</v>
       </c>
@@ -34563,7 +34563,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="539" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A539" s="4">
         <v>1829</v>
       </c>
@@ -34600,7 +34600,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="540" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A540" s="4">
         <v>1830</v>
       </c>
@@ -34637,7 +34637,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="541" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="541" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A541" s="4">
         <v>1831</v>
       </c>
@@ -34684,7 +34684,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="542" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="542" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A542" s="4">
         <v>1832</v>
       </c>
@@ -34731,7 +34731,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="543" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A543" s="4">
         <v>1833</v>
       </c>
@@ -34776,7 +34776,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="544" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A544" s="4">
         <v>1834</v>
       </c>
@@ -34823,7 +34823,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="545" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A545" s="4">
         <v>1835</v>
       </c>
@@ -34870,7 +34870,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="546" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A546" s="4">
         <v>1836</v>
       </c>
@@ -34917,7 +34917,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="547" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A547" s="4">
         <v>1837</v>
       </c>
@@ -35001,7 +35001,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="549" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A549" s="4">
         <v>1839</v>
       </c>
@@ -35048,7 +35048,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="550" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A550" s="4">
         <v>1840</v>
       </c>
@@ -35126,7 +35126,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="552" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A552" s="4">
         <v>1842</v>
       </c>
@@ -35163,7 +35163,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="553" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A553" s="4">
         <v>1843</v>
       </c>
@@ -35241,7 +35241,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="555" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A555" s="4">
         <v>1845</v>
       </c>
@@ -35280,7 +35280,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="556" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A556" s="4">
         <v>1846</v>
       </c>
@@ -35358,7 +35358,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="558" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A558" s="4">
         <v>1848</v>
       </c>
@@ -35444,7 +35444,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="560" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="560" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A560" s="4">
         <v>1850</v>
       </c>
@@ -35485,7 +35485,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="561" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A561" s="4">
         <v>1851</v>
       </c>
@@ -35532,7 +35532,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="562" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="562" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A562" s="4">
         <v>1852</v>
       </c>
@@ -35571,7 +35571,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="563" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="563" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A563" s="4">
         <v>1853</v>
       </c>
@@ -35614,7 +35614,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="564" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="564" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A564" s="4">
         <v>1854</v>
       </c>
@@ -35655,7 +35655,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="565" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="565" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A565" s="4">
         <v>1855</v>
       </c>
@@ -35702,7 +35702,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="566" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="566" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A566" s="4">
         <v>1856</v>
       </c>
@@ -35749,7 +35749,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="567" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="567" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A567" s="4">
         <v>1857</v>
       </c>
@@ -35788,7 +35788,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="568" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="568" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A568" s="4">
         <v>1858</v>
       </c>
@@ -35882,7 +35882,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="570" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="570" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A570" s="4">
         <v>1860</v>
       </c>
@@ -35929,7 +35929,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="571" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="571" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A571" s="4">
         <v>1861</v>
       </c>
@@ -35976,7 +35976,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="572" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="572" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A572" s="4">
         <v>1862</v>
       </c>
@@ -36019,7 +36019,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="573" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="573" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A573" s="4">
         <v>1863</v>
       </c>
@@ -36066,7 +36066,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="574" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="574" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A574" s="4">
         <v>1864</v>
       </c>
@@ -36111,7 +36111,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="575" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="575" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A575" s="4">
         <v>1865</v>
       </c>
@@ -36158,7 +36158,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="576" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="576" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A576" s="4">
         <v>1866</v>
       </c>
@@ -36205,7 +36205,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="577" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="577" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A577" s="4">
         <v>1867</v>
       </c>
@@ -36252,7 +36252,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="578" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A578" s="4">
         <v>1868</v>
       </c>
@@ -36299,7 +36299,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="579" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="579" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A579" s="4">
         <v>1869</v>
       </c>
@@ -36346,7 +36346,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="580" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A580" s="4">
         <v>1870</v>
       </c>
@@ -36393,7 +36393,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="581" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A581" s="4">
         <v>1871</v>
       </c>
@@ -36438,7 +36438,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="582" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A582" s="4">
         <v>1872</v>
       </c>
@@ -36483,7 +36483,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="583" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="583" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A583" s="4">
         <v>1873</v>
       </c>
@@ -36524,7 +36524,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="584" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A584" s="4">
         <v>1874</v>
       </c>
@@ -36600,7 +36600,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="586" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A586" s="4">
         <v>1876</v>
       </c>
@@ -36637,7 +36637,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="587" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="587" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A587" s="4">
         <v>1877</v>
       </c>
@@ -36684,7 +36684,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="588" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="588" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A588" s="4">
         <v>1878</v>
       </c>
@@ -36776,7 +36776,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="590" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="590" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A590" s="4">
         <v>1880</v>
       </c>
@@ -36823,7 +36823,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="591" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="591" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A591" s="4">
         <v>1881</v>
       </c>
@@ -36909,7 +36909,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="593" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="593" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A593" s="4">
         <v>1883</v>
       </c>
@@ -36956,7 +36956,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="594" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="594" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A594" s="4">
         <v>1884</v>
       </c>
@@ -37003,7 +37003,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="595" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="595" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A595" s="4">
         <v>1885</v>
       </c>
@@ -37050,7 +37050,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="596" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="596" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A596" s="4">
         <v>1886</v>
       </c>
@@ -37097,7 +37097,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="597" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="597" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A597" s="4">
         <v>1887</v>
       </c>
@@ -37144,7 +37144,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="598" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="598" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A598" s="4">
         <v>1888</v>
       </c>
@@ -37189,7 +37189,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="599" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="599" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A599" s="4">
         <v>1889</v>
       </c>
@@ -37236,7 +37236,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="600" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="600" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A600" s="4">
         <v>1890</v>
       </c>
@@ -37281,7 +37281,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="601" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="601" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A601" s="4">
         <v>1891</v>
       </c>
@@ -37318,7 +37318,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="602" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="602" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A602" s="4">
         <v>1892</v>
       </c>
@@ -37359,7 +37359,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="603" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="603" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A603" s="4">
         <v>1893</v>
       </c>
@@ -37396,7 +37396,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="604" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="604" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A604" s="4">
         <v>1894</v>
       </c>
@@ -37441,7 +37441,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="605" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="605" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A605" s="4">
         <v>1895</v>
       </c>
@@ -37488,7 +37488,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="606" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="606" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A606" s="4">
         <v>1896</v>
       </c>
@@ -37533,7 +37533,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="607" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="607" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A607" s="4">
         <v>1897</v>
       </c>
@@ -37580,7 +37580,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="608" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="608" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A608" s="4">
         <v>1898</v>
       </c>
@@ -37627,7 +37627,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="609" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="609" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A609" s="4">
         <v>1899</v>
       </c>
@@ -37719,7 +37719,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="611" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="611" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A611" s="4">
         <v>1901</v>
       </c>
@@ -37760,7 +37760,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="612" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="612" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A612" s="4">
         <v>1902</v>
       </c>
@@ -37799,7 +37799,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="613" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="613" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A613" s="4">
         <v>1903</v>
       </c>
@@ -37844,7 +37844,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="614" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="614" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A614" s="4">
         <v>1904</v>
       </c>
@@ -37889,7 +37889,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="615" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="615" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A615" s="4">
         <v>1905</v>
       </c>
@@ -37930,7 +37930,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="616" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="616" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A616" s="4">
         <v>1906</v>
       </c>
@@ -37971,7 +37971,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="617" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="617" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A617" s="4">
         <v>1907</v>
       </c>
@@ -38014,7 +38014,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="618" spans="1:15" s="31" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="618" spans="1:15" s="31" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A618" s="26">
         <v>1908</v>
       </c>
@@ -38057,7 +38057,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="619" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="619" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A619" s="4">
         <v>1909</v>
       </c>
@@ -38102,7 +38102,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="620" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="620" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A620" s="4">
         <v>1910</v>
       </c>
@@ -38147,7 +38147,7 @@
         <v>2987</v>
       </c>
     </row>
-    <row r="621" spans="1:15" s="2" customFormat="1" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="621" spans="1:15" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A621" s="4">
         <v>1911</v>
       </c>
@@ -38199,13 +38199,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O621" xr:uid="{3DDD6B5C-CAB7-4E5A-9A83-AB3221945E1E}">
-    <filterColumn colId="14">
-      <filters>
-        <filter val="VII - BEFORE - PASSED OUT"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:O621" xr:uid="{3DDD6B5C-CAB7-4E5A-9A83-AB3221945E1E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N621">
     <sortCondition ref="A2:A621"/>
   </sortState>

</xml_diff>